<commit_message>
initial commit for refactoring branch
</commit_message>
<xml_diff>
--- a/filters/Filter_BZ011.xlsx
+++ b/filters/Filter_BZ011.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e.verweyen\Desktop\Python\Pythonkram\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Software\Python\PycharmProjects\rdm_workshop\filters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C16F7B3D-8826-4121-A675-AA7FD5359F3F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19DB55A6-EFA0-4E92-8385-99BBD428C22A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,9 +26,6 @@
     <t>Kommentar</t>
   </si>
   <si>
-    <t>Datum / Uhrzeit</t>
-  </si>
-  <si>
     <t>Set aktuell</t>
   </si>
   <si>
@@ -321,6 +318,9 @@
   </si>
   <si>
     <t>Für Troubleshooting bzw. Übersicht ob der Versuch Ordnungsgemäß lief bitte die 2 auswählen bei Drücken etc.</t>
+  </si>
+  <si>
+    <t>Datum</t>
   </si>
 </sst>
 </file>
@@ -1164,23 +1164,23 @@
   <dimension ref="A1:C66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>13</v>
       </c>
@@ -1188,10 +1188,10 @@
         <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>16</v>
       </c>
@@ -1199,10 +1199,10 @@
         <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>22</v>
       </c>
@@ -1210,10 +1210,10 @@
         <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>28</v>
       </c>
@@ -1221,10 +1221,10 @@
         <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>31</v>
       </c>
@@ -1232,10 +1232,10 @@
         <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>37</v>
       </c>
@@ -1243,10 +1243,10 @@
         <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>43</v>
       </c>
@@ -1254,10 +1254,10 @@
         <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>46</v>
       </c>
@@ -1265,10 +1265,10 @@
         <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>52</v>
       </c>
@@ -1276,10 +1276,10 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>58</v>
       </c>
@@ -1287,10 +1287,10 @@
         <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>61</v>
       </c>
@@ -1298,10 +1298,10 @@
         <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>67</v>
       </c>
@@ -1309,10 +1309,10 @@
         <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>73</v>
       </c>
@@ -1320,10 +1320,10 @@
         <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>76</v>
       </c>
@@ -1331,10 +1331,10 @@
         <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>82</v>
       </c>
@@ -1342,10 +1342,10 @@
         <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>88</v>
       </c>
@@ -1353,10 +1353,10 @@
         <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>91</v>
       </c>
@@ -1364,10 +1364,10 @@
         <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>97</v>
       </c>
@@ -1375,10 +1375,10 @@
         <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>103</v>
       </c>
@@ -1386,10 +1386,10 @@
         <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>106</v>
       </c>
@@ -1397,10 +1397,10 @@
         <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>112</v>
       </c>
@@ -1408,10 +1408,10 @@
         <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>141</v>
       </c>
@@ -1419,10 +1419,10 @@
         <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>142</v>
       </c>
@@ -1430,10 +1430,10 @@
         <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>143</v>
       </c>
@@ -1441,10 +1441,10 @@
         <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>144</v>
       </c>
@@ -1452,10 +1452,10 @@
         <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>145</v>
       </c>
@@ -1463,10 +1463,10 @@
         <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>146</v>
       </c>
@@ -1474,10 +1474,10 @@
         <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>147</v>
       </c>
@@ -1485,10 +1485,10 @@
         <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>148</v>
       </c>
@@ -1496,10 +1496,10 @@
         <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>149</v>
       </c>
@@ -1507,10 +1507,10 @@
         <v>10</v>
       </c>
       <c r="C31" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>150</v>
       </c>
@@ -1518,10 +1518,10 @@
         <v>10</v>
       </c>
       <c r="C32" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>151</v>
       </c>
@@ -1529,10 +1529,10 @@
         <v>10</v>
       </c>
       <c r="C33" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>179</v>
       </c>
@@ -1540,10 +1540,10 @@
         <v>30</v>
       </c>
       <c r="C34" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>182</v>
       </c>
@@ -1551,10 +1551,10 @@
         <v>30</v>
       </c>
       <c r="C35" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>188</v>
       </c>
@@ -1562,10 +1562,10 @@
         <v>30</v>
       </c>
       <c r="C36" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>194</v>
       </c>
@@ -1573,10 +1573,10 @@
         <v>30</v>
       </c>
       <c r="C37" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>197</v>
       </c>
@@ -1584,10 +1584,10 @@
         <v>30</v>
       </c>
       <c r="C38" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>203</v>
       </c>
@@ -1595,10 +1595,10 @@
         <v>30</v>
       </c>
       <c r="C39" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>209</v>
       </c>
@@ -1606,10 +1606,10 @@
         <v>30</v>
       </c>
       <c r="C40" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>212</v>
       </c>
@@ -1617,10 +1617,10 @@
         <v>30</v>
       </c>
       <c r="C41" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>218</v>
       </c>
@@ -1628,10 +1628,10 @@
         <v>30</v>
       </c>
       <c r="C42" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>224</v>
       </c>
@@ -1639,10 +1639,10 @@
         <v>30</v>
       </c>
       <c r="C43" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>227</v>
       </c>
@@ -1650,10 +1650,10 @@
         <v>30</v>
       </c>
       <c r="C44" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>233</v>
       </c>
@@ -1661,10 +1661,10 @@
         <v>30</v>
       </c>
       <c r="C45" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>239</v>
       </c>
@@ -1672,10 +1672,10 @@
         <v>30</v>
       </c>
       <c r="C46" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>242</v>
       </c>
@@ -1683,10 +1683,10 @@
         <v>30</v>
       </c>
       <c r="C47" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>248</v>
       </c>
@@ -1694,10 +1694,10 @@
         <v>30</v>
       </c>
       <c r="C48" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>254</v>
       </c>
@@ -1705,10 +1705,10 @@
         <v>30</v>
       </c>
       <c r="C49" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>257</v>
       </c>
@@ -1716,10 +1716,10 @@
         <v>30</v>
       </c>
       <c r="C50" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>263</v>
       </c>
@@ -1727,10 +1727,10 @@
         <v>30</v>
       </c>
       <c r="C51" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>269</v>
       </c>
@@ -1738,10 +1738,10 @@
         <v>30</v>
       </c>
       <c r="C52" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>272</v>
       </c>
@@ -1749,10 +1749,10 @@
         <v>30</v>
       </c>
       <c r="C53" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>278</v>
       </c>
@@ -1760,10 +1760,10 @@
         <v>30</v>
       </c>
       <c r="C54" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>300</v>
       </c>
@@ -1771,10 +1771,10 @@
         <v>30</v>
       </c>
       <c r="C55" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>307</v>
       </c>
@@ -1782,10 +1782,10 @@
         <v>10</v>
       </c>
       <c r="C56" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>308</v>
       </c>
@@ -1793,10 +1793,10 @@
         <v>10</v>
       </c>
       <c r="C57" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>309</v>
       </c>
@@ -1804,10 +1804,10 @@
         <v>10</v>
       </c>
       <c r="C58" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>310</v>
       </c>
@@ -1815,10 +1815,10 @@
         <v>10</v>
       </c>
       <c r="C59" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>311</v>
       </c>
@@ -1826,10 +1826,10 @@
         <v>10</v>
       </c>
       <c r="C60" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>312</v>
       </c>
@@ -1837,10 +1837,10 @@
         <v>10</v>
       </c>
       <c r="C61" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>313</v>
       </c>
@@ -1848,10 +1848,10 @@
         <v>10</v>
       </c>
       <c r="C62" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>314</v>
       </c>
@@ -1859,10 +1859,10 @@
         <v>10</v>
       </c>
       <c r="C63" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>315</v>
       </c>
@@ -1870,10 +1870,10 @@
         <v>10</v>
       </c>
       <c r="C64" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>316</v>
       </c>
@@ -1881,10 +1881,10 @@
         <v>10</v>
       </c>
       <c r="C65" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>317</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>10</v>
       </c>
       <c r="C66" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1904,382 +1904,380 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CO5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="21" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="13" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="5.5546875" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="14" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="18" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="20" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="19" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="66" max="71" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="66" max="71" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="75" max="75" width="12" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="87" max="87" width="14" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s">
         <v>63</v>
       </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" t="s">
+        <v>16</v>
+      </c>
+      <c r="U1" t="s">
+        <v>17</v>
+      </c>
+      <c r="V1" t="s">
         <v>64</v>
       </c>
-      <c r="N1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" t="s">
-        <v>16</v>
-      </c>
-      <c r="T1" t="s">
-        <v>17</v>
-      </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
+        <v>65</v>
+      </c>
+      <c r="X1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" t="s">
-        <v>65</v>
-      </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>66</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>19</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AQ1" t="s">
         <v>67</v>
       </c>
-      <c r="Z1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AP1" t="s">
+      <c r="AR1" t="s">
         <v>36</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AS1" t="s">
         <v>68</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AT1" t="s">
         <v>37</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AU1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AZ1" t="s">
         <v>69</v>
       </c>
-      <c r="AT1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AY1" t="s">
+      <c r="BA1" t="s">
+        <v>70</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BC1" t="s">
         <v>43</v>
       </c>
-      <c r="AZ1" t="s">
-        <v>70</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>71</v>
-      </c>
-      <c r="BB1" t="s">
+      <c r="BD1" t="s">
+        <v>44</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>45</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>46</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>47</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>48</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>49</v>
+      </c>
+      <c r="BJ1" t="s">
         <v>72</v>
       </c>
-      <c r="BC1" t="s">
-        <v>44</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>45</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>46</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>47</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>48</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>49</v>
-      </c>
-      <c r="BI1" t="s">
+      <c r="BK1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BM1" t="s">
         <v>50</v>
       </c>
-      <c r="BJ1" t="s">
-        <v>73</v>
-      </c>
-      <c r="BK1" t="s">
-        <v>74</v>
-      </c>
-      <c r="BL1" t="s">
+      <c r="BN1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BT1" t="s">
         <v>75</v>
       </c>
-      <c r="BM1" t="s">
-        <v>51</v>
-      </c>
-      <c r="BN1" t="s">
-        <v>52</v>
-      </c>
-      <c r="BO1" t="s">
-        <v>53</v>
-      </c>
-      <c r="BP1" t="s">
-        <v>54</v>
-      </c>
-      <c r="BQ1" t="s">
-        <v>55</v>
-      </c>
-      <c r="BR1" t="s">
-        <v>56</v>
-      </c>
-      <c r="BS1" t="s">
+      <c r="BU1" t="s">
         <v>57</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BV1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BY1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BZ1" t="s">
         <v>76</v>
       </c>
-      <c r="BU1" t="s">
-        <v>58</v>
-      </c>
-      <c r="BV1" t="s">
-        <v>59</v>
-      </c>
-      <c r="BW1" t="s">
-        <v>60</v>
-      </c>
-      <c r="BX1" t="s">
-        <v>61</v>
-      </c>
-      <c r="BY1" t="s">
-        <v>62</v>
-      </c>
-      <c r="BZ1" t="s">
+      <c r="CA1" t="s">
         <v>77</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CB1" t="s">
         <v>78</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CC1" t="s">
         <v>79</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="CD1" t="s">
         <v>80</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="CE1" t="s">
         <v>81</v>
       </c>
-      <c r="CE1" t="s">
+      <c r="CF1" t="s">
         <v>82</v>
       </c>
-      <c r="CF1" t="s">
+      <c r="CG1" t="s">
         <v>83</v>
       </c>
-      <c r="CG1" t="s">
+      <c r="CH1" t="s">
         <v>84</v>
       </c>
-      <c r="CH1" t="s">
+      <c r="CI1" t="s">
         <v>85</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="CJ1" t="s">
         <v>86</v>
       </c>
-      <c r="CJ1" t="s">
+      <c r="CK1" t="s">
         <v>87</v>
       </c>
-      <c r="CK1" t="s">
+      <c r="CL1" t="s">
         <v>88</v>
       </c>
-      <c r="CL1" t="s">
+      <c r="CM1" t="s">
         <v>89</v>
       </c>
-      <c r="CM1" t="s">
+      <c r="CN1" t="s">
         <v>90</v>
       </c>
-      <c r="CN1" t="s">
+      <c r="CO1" t="s">
         <v>91</v>
       </c>
-      <c r="CO1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:93" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2560,14 +2558,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:93" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>